<commit_message>
Fix Excel formatting: Increase row heights for long text
</commit_message>
<xml_diff>
--- a/Chargeback_Explanation_Form_v2.xlsx
+++ b/Chargeback_Explanation_Form_v2.xlsx
@@ -507,7 +507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C32"/>
+  <dimension ref="B2:C22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,7 +549,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="60" customHeight="1">
+    <row r="8" ht="90" customHeight="1">
       <c r="B8" s="5" t="inlineStr">
         <is>
           <t>[   ]</t>
@@ -562,7 +562,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="60" customHeight="1">
+    <row r="9" ht="90" customHeight="1">
       <c r="B9" s="5" t="inlineStr">
         <is>
           <t>[   ]</t>
@@ -575,7 +575,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="60" customHeight="1">
+    <row r="10" ht="90" customHeight="1">
       <c r="B10" s="5" t="inlineStr">
         <is>
           <t>[   ]</t>
@@ -588,7 +588,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="60" customHeight="1">
+    <row r="11" ht="90" customHeight="1">
       <c r="B11" s="5" t="inlineStr">
         <is>
           <t>[   ]</t>
@@ -601,7 +601,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="60" customHeight="1">
+    <row r="12" ht="90" customHeight="1">
       <c r="B12" s="5" t="inlineStr">
         <is>
           <t>[   ]</t>
@@ -635,7 +635,7 @@
         </is>
       </c>
     </row>
-    <row r="22">
+    <row r="22" ht="450" customHeight="1">
       <c r="B22" s="6" t="inlineStr">
         <is>
           <t>For VIP purchases
@@ -653,16 +653,6 @@
         </is>
       </c>
     </row>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B21:C21"/>
@@ -670,8 +660,8 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B14:C19"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B22:C32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>